<commit_message>
worked on BOM, not complete
</commit_message>
<xml_diff>
--- a/Documentation/BOM/BOM.xlsx
+++ b/Documentation/BOM/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\OneDrive\Documents\GitHub\GimbalBoard_Hardware\Documentation\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kilian\Github\GimbalBoard_Hardware\Documentation\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB37BFD0-969C-46FB-BD9A-41848558392B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D51F36D-48FB-46E9-B9FB-632442E7FA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4608" yWindow="1560" windowWidth="16608" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>Id</t>
   </si>
@@ -132,6 +132,87 @@
   </si>
   <si>
     <t>toggle switch</t>
+  </si>
+  <si>
+    <t>AndersonPP</t>
+  </si>
+  <si>
+    <t>Zener Diode</t>
+  </si>
+  <si>
+    <t>330 Resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 Resistor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">43 Resistor </t>
+  </si>
+  <si>
+    <t>0.1uF Capacitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teensy </t>
+  </si>
+  <si>
+    <t>510 Resistor</t>
+  </si>
+  <si>
+    <t>Molex Connectors</t>
+  </si>
+  <si>
+    <t>ESR03EZPJ331</t>
+  </si>
+  <si>
+    <t>Digi-key</t>
+  </si>
+  <si>
+    <t>ESR03EZPJ511</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/ESR03EZPJ101/1983452</t>
+  </si>
+  <si>
+    <t>ESR03EZPJ101</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/ESR03EZPJ511/1762937</t>
+  </si>
+  <si>
+    <t>ESR10EZPJ430</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/ESR10EZPJ430/1762819</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/ESR03EZPJ331/1762730</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL10B104KO8NNNC/3889091</t>
+  </si>
+  <si>
+    <t>CL10B104KO8NNNC</t>
+  </si>
+  <si>
+    <t>OKI 5V</t>
+  </si>
+  <si>
+    <t>OKI-78SR-5/1.5-W36H-C</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-power-solutions-inc/OKI-78SR-5-1.5-W36H-C/3438675</t>
+  </si>
+  <si>
+    <t>OKI 3.3V</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-power-solutions-inc/OKI-78SR-3.3-1.5-W36H-C/4878851</t>
+  </si>
+  <si>
+    <t>OKI-78SR-3.3/1.5-W36H-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digi-key </t>
   </si>
 </sst>
 </file>
@@ -508,20 +589,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="12.6328125" customWidth="1"/>
-    <col min="6" max="6" width="22.6328125" customWidth="1"/>
-    <col min="7" max="10" width="12.6328125" customWidth="1"/>
+    <col min="1" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="7" max="10" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,7 +637,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E2" t="s">
         <v>10</v>
       </c>
@@ -576,7 +657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
         <v>14</v>
       </c>
@@ -596,7 +677,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
         <v>18</v>
       </c>
@@ -616,7 +697,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
         <v>27</v>
       </c>
@@ -624,7 +705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
         <v>26</v>
       </c>
@@ -644,7 +725,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
         <v>28</v>
       </c>
@@ -664,7 +745,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
         <v>32</v>
       </c>
@@ -678,9 +759,181 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="I12">
+        <v>0.1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>0.1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14">
+        <v>9</v>
+      </c>
+      <c r="I14">
+        <v>0.1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15">
+        <v>11</v>
+      </c>
+      <c r="I15">
+        <v>0.1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0.1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>4.3</v>
+      </c>
+      <c r="J19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>4.3</v>
+      </c>
+      <c r="J20" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new connectors and decals
i have the 3x2 molex on here as well as some cowboy bebop decals.
the swtich still needs be confirmed.
</commit_message>
<xml_diff>
--- a/Documentation/BOM/BOM.xlsx
+++ b/Documentation/BOM/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\OneDrive\Documents\GitHub\GimbalBoard_Hardware\Documentation\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8AEE71-CB43-4BE5-BAAE-B52951EF8928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F0B669-01D0-47BC-8945-EFCD645FA70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>Id</t>
   </si>
@@ -119,27 +119,15 @@
     <t>dual NMOS</t>
   </si>
   <si>
-    <t>digikey</t>
-  </si>
-  <si>
     <t>2N7002NCT-ND</t>
   </si>
   <si>
     <t>https://www.newark.com/on-semiconductor/2n7002/mosfet-n-channel-60v-115ma-sot/dp/58K9651?gclid=CjwKCAiAm7OMBhAQEiwArvGi3JAKS1RbplkHNRLcR4XTUiYGfFYLS7X2EdIIIidl7Vz5AOVoCz_QBRoCotQQAvD_BwE&amp;mckv=s_dc|pcrid|502765332365|plid||kword|2n7002|match|p|slid||product||pgrid|118037913589|ptaid|kwd-713885255|&amp;cmp=KNC-GUSA-GEN-SKU-Semiconductors-Semiconductors-https://www.newark.com/on-semiconductor/2n7002/mosfet-n-channel-60v-115ma-sot/dp/58K9651?gclid=CjwKCAiAm7OMBhAQEiwArvGi3JAKS1RbplkHNRLcR4XTUiYGfFYLS7X2EdIIIidl7Vz5AOVoCz_QBRoCotQQAvD_BwE&amp;mckv=s_dc|pcrid|502765332365|plid||kword|2n7002|match|p|slid||product||pgrid|118037913589|ptaid|kwd-713885255|&amp;cmp=KNC-GUSA-GEN-SKU-Semiconductors-Semiconductors-Discretes</t>
   </si>
   <si>
-    <t>pb-smd</t>
-  </si>
-  <si>
-    <t>toggle switch</t>
-  </si>
-  <si>
     <t>AndersonPP</t>
   </si>
   <si>
-    <t>Zener Diode</t>
-  </si>
-  <si>
     <t>330 Resistor</t>
   </si>
   <si>
@@ -212,10 +200,7 @@
     <t xml:space="preserve">Digi-key </t>
   </si>
   <si>
-    <t>Molex Connectors (horizontal)</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/KDZVTFTR3-9B/9697263</t>
+    <t>Molex Connectors (horizontal) 3x2</t>
   </si>
 </sst>
 </file>
@@ -595,7 +580,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -724,7 +709,7 @@
       <c r="I6">
         <v>0.48</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -733,7 +718,7 @@
         <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
         <v>12</v>
@@ -745,56 +730,29 @@
         <v>0.34</v>
       </c>
       <c r="J7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H10">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11">
-        <v>2</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>61</v>
-      </c>
+      <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H12">
         <v>8</v>
@@ -802,19 +760,19 @@
       <c r="I12">
         <v>0.1</v>
       </c>
-      <c r="J12" t="s">
-        <v>47</v>
+      <c r="J12" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G13" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H13">
         <v>2</v>
@@ -823,18 +781,18 @@
         <v>0.1</v>
       </c>
       <c r="J13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E14" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H14">
         <v>9</v>
@@ -843,18 +801,18 @@
         <v>0.1</v>
       </c>
       <c r="J14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H15">
         <v>11</v>
@@ -863,18 +821,18 @@
         <v>0.1</v>
       </c>
       <c r="J15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -882,13 +840,13 @@
       <c r="I16">
         <v>0.1</v>
       </c>
-      <c r="J16" t="s">
-        <v>51</v>
+      <c r="J16" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -896,21 +854,21 @@
     </row>
     <row r="18" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E18" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H18">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G19" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H19">
         <v>2</v>
@@ -919,18 +877,18 @@
         <v>4.3</v>
       </c>
       <c r="J19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E20" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G20" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -939,7 +897,7 @@
         <v>4.3</v>
       </c>
       <c r="J20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -948,9 +906,11 @@
     <hyperlink ref="J3" r:id="rId2" xr:uid="{507B4305-BFFF-48C6-9F4C-3D18E536E630}"/>
     <hyperlink ref="J4" r:id="rId3" xr:uid="{E9A7265F-97A5-498D-A0CF-D77DBB3EEB0A}"/>
     <hyperlink ref="K1" r:id="rId4" location="gid=1677207111" xr:uid="{4DD69053-3FD8-49A6-9DCA-4487FA9826BA}"/>
-    <hyperlink ref="J11" r:id="rId5" xr:uid="{0C77E8FC-751A-447F-9F41-46CCC889FCE6}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{DB6055C9-403F-4FF7-B11B-232C45C97DD4}"/>
+    <hyperlink ref="J12" r:id="rId6" xr:uid="{BFBD83AA-CC2A-4A34-B667-1DA06B7AFBC8}"/>
+    <hyperlink ref="J16" r:id="rId7" xr:uid="{A9AFF38B-2117-43AA-BCF0-717D751E2BB1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
the correct switch, and some decals
some decals and the correct switch
</commit_message>
<xml_diff>
--- a/Documentation/BOM/BOM.xlsx
+++ b/Documentation/BOM/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\OneDrive\Documents\GitHub\GimbalBoard_Hardware\Documentation\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F0B669-01D0-47BC-8945-EFCD645FA70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910EEF3A-D838-4AFE-99FE-F8639724BBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -580,7 +580,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>